<commit_message>
added supportport for tutor names rather than exclusively student ID
</commit_message>
<xml_diff>
--- a/Sample Data/Fall2017AvailabilitySubjects.xlsx
+++ b/Sample Data/Fall2017AvailabilitySubjects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samberling/OneDrive/School/Spring 2018/CSCI 440/Schedule Generator/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67F50DD-E7C5-A548-904E-85128B8905D0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814A5100-AD5B-5E45-9BE8-E10EC47BDC6C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16840" yWindow="460" windowWidth="16760" windowHeight="19180" xr2:uid="{71D515E7-43FC-794D-8CCB-B2803B57DA0E}"/>
   </bookViews>
@@ -207,129 +207,6 @@
     <t>5-14</t>
   </si>
   <si>
-    <t>mzach</t>
-  </si>
-  <si>
-    <t>jdejesus</t>
-  </si>
-  <si>
-    <t>iyu</t>
-  </si>
-  <si>
-    <t>eparlan</t>
-  </si>
-  <si>
-    <t>bwitter</t>
-  </si>
-  <si>
-    <t>gchang</t>
-  </si>
-  <si>
-    <t>jli</t>
-  </si>
-  <si>
-    <t>kstutz</t>
-  </si>
-  <si>
-    <t>klamar</t>
-  </si>
-  <si>
-    <t>sberling</t>
-  </si>
-  <si>
-    <t>mkraus</t>
-  </si>
-  <si>
-    <t>glizier</t>
-  </si>
-  <si>
-    <t>cvanboven</t>
-  </si>
-  <si>
-    <t>lroberts</t>
-  </si>
-  <si>
-    <t>zbranch</t>
-  </si>
-  <si>
-    <t>mpoplawsky</t>
-  </si>
-  <si>
-    <t>kmoffett</t>
-  </si>
-  <si>
-    <t>bimada</t>
-  </si>
-  <si>
-    <t>rchaiser</t>
-  </si>
-  <si>
-    <t>mberrens</t>
-  </si>
-  <si>
-    <t>jfonseca</t>
-  </si>
-  <si>
-    <t>kmiller</t>
-  </si>
-  <si>
-    <t>jholgate</t>
-  </si>
-  <si>
-    <t>asalado</t>
-  </si>
-  <si>
-    <t>jhutcheson</t>
-  </si>
-  <si>
-    <t>ctomkins</t>
-  </si>
-  <si>
-    <t>esmith</t>
-  </si>
-  <si>
-    <t>iamaya</t>
-  </si>
-  <si>
-    <t>ianderson</t>
-  </si>
-  <si>
-    <t>lbengtson</t>
-  </si>
-  <si>
-    <t>adiaz</t>
-  </si>
-  <si>
-    <t>tgill</t>
-  </si>
-  <si>
-    <t>akabir</t>
-  </si>
-  <si>
-    <t>hkatz</t>
-  </si>
-  <si>
-    <t>wkeyse</t>
-  </si>
-  <si>
-    <t>rlaitila</t>
-  </si>
-  <si>
-    <t>aluong</t>
-  </si>
-  <si>
-    <t>lmorton</t>
-  </si>
-  <si>
-    <t>smyers</t>
-  </si>
-  <si>
-    <t>mtaponga</t>
-  </si>
-  <si>
-    <t>swalling</t>
-  </si>
-  <si>
     <t>Accounting &amp; Finance</t>
   </si>
   <si>
@@ -382,6 +259,129 @@
   </si>
   <si>
     <t>Statistics</t>
+  </si>
+  <si>
+    <t>mzach|Maggie Zach</t>
+  </si>
+  <si>
+    <t>jdejesus|James DeJesus</t>
+  </si>
+  <si>
+    <t>iyu|Ivin Yu</t>
+  </si>
+  <si>
+    <t>eparlan|Emily Parlan</t>
+  </si>
+  <si>
+    <t>bwitter|Brynn Witter</t>
+  </si>
+  <si>
+    <t>gchang|Gabby Chang</t>
+  </si>
+  <si>
+    <t>jli|Jiawen Li</t>
+  </si>
+  <si>
+    <t>kstutz|Kathryn Stutz</t>
+  </si>
+  <si>
+    <t>klamar|Kara Ann Lamar</t>
+  </si>
+  <si>
+    <t>sberling|Sam Berling</t>
+  </si>
+  <si>
+    <t>mkraus|Miranda Kraus</t>
+  </si>
+  <si>
+    <t>glizier|Geremia Lizier-Zmudzinksi</t>
+  </si>
+  <si>
+    <t>cvanboven|Caleb van Boven</t>
+  </si>
+  <si>
+    <t>lroberts|Lindsey Roberts</t>
+  </si>
+  <si>
+    <t>zbranch|Zoe Branch</t>
+  </si>
+  <si>
+    <t>mpoplawsky|Meadow Poplawsky</t>
+  </si>
+  <si>
+    <t>kmoffett|Katarina Moffett</t>
+  </si>
+  <si>
+    <t>bimada|Brittney Imada</t>
+  </si>
+  <si>
+    <t>rchaiser|Rachel Chaiser</t>
+  </si>
+  <si>
+    <t>mberrens|Maggie Berrens</t>
+  </si>
+  <si>
+    <t>jfonseca|Jordan Fonseca</t>
+  </si>
+  <si>
+    <t>kmiller|Kyle Miller</t>
+  </si>
+  <si>
+    <t>jholgate|Jule Holgate</t>
+  </si>
+  <si>
+    <t>asalado|Arcelia Salado Alvarado</t>
+  </si>
+  <si>
+    <t>jhutechson|Jayne Hutcheson</t>
+  </si>
+  <si>
+    <t>ctomkins|Cole Tomkins</t>
+  </si>
+  <si>
+    <t>esmith|Erika Smith</t>
+  </si>
+  <si>
+    <t>iamaya|Isabel Amaya</t>
+  </si>
+  <si>
+    <t>ianderson|Isabelle Anderson</t>
+  </si>
+  <si>
+    <t>lbengston|Lilly Bengston</t>
+  </si>
+  <si>
+    <t>adiaz|Amanda Diaz</t>
+  </si>
+  <si>
+    <t>tgill|Tiare Gill</t>
+  </si>
+  <si>
+    <t>akabir|Alia Kabir</t>
+  </si>
+  <si>
+    <t>hkatz|Hannah Katz</t>
+  </si>
+  <si>
+    <t>wkeyse|William Keyse</t>
+  </si>
+  <si>
+    <t>rlaitila|Rachael Laitila</t>
+  </si>
+  <si>
+    <t>aluong|Amy Luong</t>
+  </si>
+  <si>
+    <t>lmorton|Lura Morton</t>
+  </si>
+  <si>
+    <t>smyers|Sophie Myers</t>
+  </si>
+  <si>
+    <t>mtapogna|Max Tapogna</t>
+  </si>
+  <si>
+    <t>swalling|Sarah Walling-Bell</t>
   </si>
 </sst>
 </file>
@@ -838,9 +838,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D71848E-EFA5-494B-8942-CEECAAF65D58}">
   <dimension ref="A1:BN43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BJ42" sqref="BJ42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AV1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1034,187 +1034,187 @@
     </row>
     <row r="2" spans="1:66">
       <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1">
+        <v>2</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>2</v>
+      </c>
+      <c r="W2" s="1">
+        <v>2</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>2</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>2</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>2</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1">
-        <v>2</v>
-      </c>
-      <c r="T2" s="1">
-        <v>2</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1">
-        <v>2</v>
-      </c>
-      <c r="W2" s="1">
-        <v>2</v>
-      </c>
-      <c r="X2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AO2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AP2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AR2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>2</v>
-      </c>
-      <c r="AV2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BA2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BB2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BC2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BE2" s="1">
-        <v>2</v>
-      </c>
-      <c r="BF2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>101</v>
       </c>
       <c r="BJ2" s="3">
         <v>8</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="3" spans="1:66">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="BI3" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="BN3">
         <v>1</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="4" spans="1:66">
       <c r="A4" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -1593,7 +1593,7 @@
         <v>1</v>
       </c>
       <c r="BI4" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="BN4">
         <v>1</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="5" spans="1:66">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1781,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="BI5" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="BN5">
         <v>1</v>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="6" spans="1:66">
       <c r="A6" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -1969,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="BI6" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="BN6">
         <v>1</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="7" spans="1:66">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -2157,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="BI7" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="BJ7" s="3">
         <v>-2</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="8" spans="1:66">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -2348,7 +2348,7 @@
         <v>2</v>
       </c>
       <c r="BI8" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="BN8">
         <v>1</v>
@@ -2356,7 +2356,7 @@
     </row>
     <row r="9" spans="1:66">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -2536,7 +2536,7 @@
         <v>1</v>
       </c>
       <c r="BI9" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="BN9">
         <v>1</v>
@@ -2544,7 +2544,7 @@
     </row>
     <row r="10" spans="1:66">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="BI10" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BJ10" s="3">
         <v>-2</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="11" spans="1:66">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -2915,7 +2915,7 @@
         <v>2</v>
       </c>
       <c r="BI11" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="BJ11" s="3">
         <v>-2</v>
@@ -2926,7 +2926,7 @@
     </row>
     <row r="12" spans="1:66">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -3106,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="BI12" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="BJ12" s="3">
         <v>-2</v>
@@ -3117,187 +3117,187 @@
     </row>
     <row r="13" spans="1:66">
       <c r="A13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2</v>
+      </c>
+      <c r="N13" s="1">
+        <v>2</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>2</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0</v>
+      </c>
+      <c r="W13" s="1">
+        <v>0</v>
+      </c>
+      <c r="X13" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AK13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AU13" s="1">
+        <v>2</v>
+      </c>
+      <c r="AV13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ13" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA13" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB13" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC13" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BE13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF13" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG13" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI13" t="s">
         <v>71</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>2</v>
-      </c>
-      <c r="I13" s="1">
-        <v>2</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1">
-        <v>2</v>
-      </c>
-      <c r="M13" s="1">
-        <v>2</v>
-      </c>
-      <c r="N13" s="1">
-        <v>2</v>
-      </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>1</v>
-      </c>
-      <c r="R13" s="1">
-        <v>1</v>
-      </c>
-      <c r="S13" s="1">
-        <v>0</v>
-      </c>
-      <c r="T13" s="1">
-        <v>2</v>
-      </c>
-      <c r="U13" s="1">
-        <v>0</v>
-      </c>
-      <c r="V13" s="1">
-        <v>0</v>
-      </c>
-      <c r="W13" s="1">
-        <v>0</v>
-      </c>
-      <c r="X13" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="1">
-        <v>2</v>
-      </c>
-      <c r="AG13" s="1">
-        <v>2</v>
-      </c>
-      <c r="AH13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="1">
-        <v>2</v>
-      </c>
-      <c r="AK13" s="1">
-        <v>2</v>
-      </c>
-      <c r="AL13" s="1">
-        <v>2</v>
-      </c>
-      <c r="AM13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AP13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT13" s="1">
-        <v>2</v>
-      </c>
-      <c r="AU13" s="1">
-        <v>2</v>
-      </c>
-      <c r="AV13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AX13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ13" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA13" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB13" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC13" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD13" s="1">
-        <v>2</v>
-      </c>
-      <c r="BE13" s="1">
-        <v>2</v>
-      </c>
-      <c r="BF13" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG13" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH13" s="1">
-        <v>2</v>
-      </c>
-      <c r="BI13" t="s">
-        <v>112</v>
       </c>
       <c r="BN13">
         <v>1</v>
@@ -3305,7 +3305,7 @@
     </row>
     <row r="14" spans="1:66">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="BI14" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="BN14">
         <v>1</v>
@@ -3493,7 +3493,7 @@
     </row>
     <row r="15" spans="1:66">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -3673,7 +3673,7 @@
         <v>0</v>
       </c>
       <c r="BI15" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="BN15">
         <v>1</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="16" spans="1:66">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -3861,10 +3861,10 @@
         <v>2</v>
       </c>
       <c r="BI16" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="BJ16" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BK16">
         <v>10</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="17" spans="1:66">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -4058,7 +4058,7 @@
         <v>2</v>
       </c>
       <c r="BI17" t="s">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="BN17">
         <v>1</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="18" spans="1:66">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -4246,7 +4246,7 @@
         <v>2</v>
       </c>
       <c r="BI18" t="s">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="BN18">
         <v>1</v>
@@ -4254,7 +4254,7 @@
     </row>
     <row r="19" spans="1:66">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -4434,7 +4434,7 @@
         <v>0</v>
       </c>
       <c r="BI19" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="BN19">
         <v>1</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="20" spans="1:66">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -4622,7 +4622,7 @@
         <v>2</v>
       </c>
       <c r="BI20" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="BN20">
         <v>1</v>
@@ -4630,7 +4630,7 @@
     </row>
     <row r="21" spans="1:66">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -4810,7 +4810,7 @@
         <v>0</v>
       </c>
       <c r="BI21" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="BN21">
         <v>1</v>
@@ -4818,7 +4818,7 @@
     </row>
     <row r="22" spans="1:66">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -4998,13 +4998,13 @@
         <v>0</v>
       </c>
       <c r="BI22" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="BJ22" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BK22" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="BL22">
         <v>12</v>
@@ -5018,7 +5018,7 @@
     </row>
     <row r="23" spans="1:66">
       <c r="A23" s="1" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -5198,7 +5198,7 @@
         <v>0</v>
       </c>
       <c r="BI23" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="BJ23" s="3">
         <v>-2</v>
@@ -5209,7 +5209,7 @@
     </row>
     <row r="24" spans="1:66">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -5389,7 +5389,7 @@
         <v>0</v>
       </c>
       <c r="BI24" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="BJ24" s="3">
         <v>-2</v>
@@ -5400,7 +5400,7 @@
     </row>
     <row r="25" spans="1:66">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -5580,7 +5580,7 @@
         <v>2</v>
       </c>
       <c r="BI25" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="BN25">
         <v>1</v>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="26" spans="1:66">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -5768,7 +5768,7 @@
         <v>1</v>
       </c>
       <c r="BI26" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="BN26">
         <v>1</v>
@@ -5776,7 +5776,7 @@
     </row>
     <row r="27" spans="1:66">
       <c r="A27" s="1" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -5956,7 +5956,7 @@
         <v>1</v>
       </c>
       <c r="BI27" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="BN27">
         <v>1</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="28" spans="1:66">
       <c r="A28" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="B28" s="1">
         <v>2</v>
@@ -6144,7 +6144,7 @@
         <v>2</v>
       </c>
       <c r="BI28" t="s">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="BJ28" s="3">
         <v>-2</v>
@@ -6155,7 +6155,7 @@
     </row>
     <row r="29" spans="1:66">
       <c r="A29" s="1" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -6335,7 +6335,7 @@
         <v>1</v>
       </c>
       <c r="BI29" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BN29">
         <v>1</v>
@@ -6343,7 +6343,7 @@
     </row>
     <row r="30" spans="1:66">
       <c r="A30" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="B30" s="1">
         <v>2</v>
@@ -6523,7 +6523,7 @@
         <v>2</v>
       </c>
       <c r="BI30" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BJ30" s="3">
         <v>9</v>
@@ -6537,7 +6537,7 @@
     </row>
     <row r="31" spans="1:66">
       <c r="A31" s="1" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -6717,10 +6717,10 @@
         <v>0</v>
       </c>
       <c r="BI31" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="BJ31" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BK31" s="4">
         <v>-2</v>
@@ -6731,7 +6731,7 @@
     </row>
     <row r="32" spans="1:66">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -6911,7 +6911,7 @@
         <v>2</v>
       </c>
       <c r="BI32" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BJ32" s="3">
         <v>-2</v>
@@ -6922,7 +6922,7 @@
     </row>
     <row r="33" spans="1:66">
       <c r="A33" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -7102,10 +7102,10 @@
         <v>0</v>
       </c>
       <c r="BI33" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BJ33" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="BK33" s="4">
         <v>12</v>
@@ -7119,7 +7119,7 @@
     </row>
     <row r="34" spans="1:66">
       <c r="A34" s="1" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B34" s="1">
         <v>2</v>
@@ -7299,7 +7299,7 @@
         <v>2</v>
       </c>
       <c r="BI34" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BN34">
         <v>1</v>
@@ -7307,7 +7307,7 @@
     </row>
     <row r="35" spans="1:66">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
@@ -7487,7 +7487,7 @@
         <v>0</v>
       </c>
       <c r="BI35" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BN35">
         <v>1</v>
@@ -7495,7 +7495,7 @@
     </row>
     <row r="36" spans="1:66">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -7675,7 +7675,7 @@
         <v>0</v>
       </c>
       <c r="BI36" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BN36">
         <v>1</v>
@@ -7683,7 +7683,7 @@
     </row>
     <row r="37" spans="1:66">
       <c r="A37" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -7863,7 +7863,7 @@
         <v>2</v>
       </c>
       <c r="BI37" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BN37">
         <v>1</v>
@@ -7871,7 +7871,7 @@
     </row>
     <row r="38" spans="1:66">
       <c r="A38" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -8051,7 +8051,7 @@
         <v>2</v>
       </c>
       <c r="BI38" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BJ38" s="3">
         <v>3</v>
@@ -8065,7 +8065,7 @@
     </row>
     <row r="39" spans="1:66">
       <c r="A39" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -8245,7 +8245,7 @@
         <v>2</v>
       </c>
       <c r="BI39" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BJ39" s="3">
         <v>12</v>
@@ -8256,7 +8256,7 @@
     </row>
     <row r="40" spans="1:66">
       <c r="A40" s="1" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
@@ -8436,10 +8436,10 @@
         <v>1</v>
       </c>
       <c r="BI40" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BJ40" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="BK40" s="4">
         <v>-2</v>
@@ -8450,7 +8450,7 @@
     </row>
     <row r="41" spans="1:66">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -8630,7 +8630,7 @@
         <v>1</v>
       </c>
       <c r="BI41" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BN41">
         <v>1</v>
@@ -8638,7 +8638,7 @@
     </row>
     <row r="42" spans="1:66">
       <c r="A42" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -8818,7 +8818,7 @@
         <v>0</v>
       </c>
       <c r="BI42" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="BN42">
         <v>1</v>
@@ -8826,239 +8826,239 @@
     </row>
     <row r="43" spans="1:66">
       <c r="B43">
-        <f>SUMIF(B2:B42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" ref="B43:AG43" si="0">SUMIF(B2:B42, "&lt;2", $BN2:$BN42)</f>
         <v>37</v>
       </c>
       <c r="C43">
-        <f>SUMIF(C2:C42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="D43">
-        <f>SUMIF(D2:D42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="E43">
-        <f>SUMIF(E2:E42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F43">
-        <f>SUMIF(F2:F42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="G43">
-        <f>SUMIF(G2:G42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="H43">
-        <f>SUMIF(H2:H42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="I43">
-        <f>SUMIF(I2:I42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="J43">
-        <f>SUMIF(J2:J42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="K43">
-        <f>SUMIF(K2:K42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="L43">
-        <f>SUMIF(L2:L42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="M43">
-        <f>SUMIF(M2:M42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="N43">
-        <f>SUMIF(N2:N42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="O43">
-        <f>SUMIF(O2:O42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="P43">
-        <f>SUMIF(P2:P42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="Q43">
-        <f>SUMIF(Q2:Q42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="R43">
-        <f>SUMIF(R2:R42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="S43">
-        <f>SUMIF(S2:S42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="T43">
-        <f>SUMIF(T2:T42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="U43">
-        <f>SUMIF(U2:U42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="V43">
-        <f>SUMIF(V2:V42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="W43">
-        <f>SUMIF(W2:W42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="X43">
-        <f>SUMIF(X2:X42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="Y43">
-        <f>SUMIF(Y2:Y42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="Z43">
-        <f>SUMIF(Z2:Z42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="AA43">
-        <f>SUMIF(AA2:AA42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="AB43">
-        <f>SUMIF(AB2:AB42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="AC43">
-        <f>SUMIF(AC2:AC42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="AD43">
-        <f>SUMIF(AD2:AD42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="AE43">
-        <f>SUMIF(AE2:AE42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="AF43">
-        <f>SUMIF(AF2:AF42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="AG43">
-        <f>SUMIF(AG2:AG42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="AH43">
-        <f>SUMIF(AH2:AH42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" ref="AH43:BM43" si="1">SUMIF(AH2:AH42, "&lt;2", $BN2:$BN42)</f>
         <v>40</v>
       </c>
       <c r="AI43">
-        <f>SUMIF(AI2:AI42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="AJ43">
-        <f>SUMIF(AJ2:AJ42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="AK43">
-        <f>SUMIF(AK2:AK42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AL43">
-        <f>SUMIF(AL2:AL42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="AM43">
-        <f>SUMIF(AM2:AM42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="AN43">
-        <f>SUMIF(AN2:AN42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="AO43">
-        <f>SUMIF(AO2:AO42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="AP43">
-        <f>SUMIF(AP2:AP42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="AQ43">
-        <f>SUMIF(AQ2:AQ42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AR43">
-        <f>SUMIF(AR2:AR42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="AS43">
-        <f>SUMIF(AS2:AS42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="AT43">
-        <f>SUMIF(AT2:AT42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="AU43">
-        <f>SUMIF(AU2:AU42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="AV43">
-        <f>SUMIF(AV2:AV42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="AW43">
-        <f>SUMIF(AW2:AW42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="AX43">
-        <f>SUMIF(AX2:AX42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="AY43">
-        <f>SUMIF(AY2:AY42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="AZ43">
-        <f>SUMIF(AZ2:AZ42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="BA43">
-        <f>SUMIF(BA2:BA42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="BB43">
-        <f>SUMIF(BB2:BB42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="BC43">
-        <f>SUMIF(BC2:BC42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="BD43">
-        <f>SUMIF(BD2:BD42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="BE43">
-        <f>SUMIF(BE2:BE42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="BF43">
-        <f>SUMIF(BF2:BF42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="BG43">
-        <f>SUMIF(BG2:BG42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="BH43">
-        <f>SUMIF(BH2:BH42, "&lt;2", $BN2:$BN42)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
     </row>

</xml_diff>